<commit_message>
Making it do stuff
</commit_message>
<xml_diff>
--- a/app/jobs.xlsx
+++ b/app/jobs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="109">
   <si>
     <t>Door Name</t>
   </si>
@@ -311,15 +311,9 @@
     <t>Waiting on EC for path and new PS</t>
   </si>
   <si>
-    <t>String to frame</t>
-  </si>
-  <si>
     <t>Waiting on EC for conduit issue</t>
   </si>
   <si>
-    <t>Waiting on EC for conduit</t>
-  </si>
-  <si>
     <t>String pulled in frame</t>
   </si>
   <si>
@@ -347,16 +341,22 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Missing EL hardware</t>
-  </si>
-  <si>
     <t>Needs Conduit, Missing EL hardware</t>
   </si>
   <si>
-    <t>Missing EL hardware, Added ADO?</t>
-  </si>
-  <si>
-    <t>Missing EL hardware, wrong hinges</t>
+    <t>Added ADO?</t>
+  </si>
+  <si>
+    <t>wrong hinges</t>
+  </si>
+  <si>
+    <t>CR needs mud ring</t>
+  </si>
+  <si>
+    <t>Have to check if powersupply is hooked up for strike</t>
+  </si>
+  <si>
+    <t>Waiting on EC for path, cable pulled to wrong location</t>
   </si>
 </sst>
 </file>
@@ -712,8 +712,8 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,7 +726,7 @@
     <col min="8" max="8" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="10" width="10.83203125" style="1"/>
     <col min="11" max="11" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="34.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -765,7 +765,7 @@
         <v>88</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -780,25 +780,25 @@
         <v>117</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L2" s="3"/>
     </row>
@@ -814,25 +814,25 @@
         <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L3" s="3"/>
     </row>
@@ -848,29 +848,27 @@
         <v>341</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -884,29 +882,27 @@
         <v>341</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -920,25 +916,25 @@
         <v>341</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L6" s="3"/>
     </row>
@@ -954,29 +950,27 @@
         <v>341</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -990,29 +984,27 @@
         <v>341</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1026,28 +1018,28 @@
         <v>341</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1062,29 +1054,27 @@
         <v>341</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1098,28 +1088,28 @@
         <v>512</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1134,28 +1124,28 @@
         <v>512</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1170,25 +1160,25 @@
         <v>314</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L13" s="3"/>
     </row>
@@ -1204,28 +1194,28 @@
         <v>314</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1238,25 +1228,25 @@
         <v>714</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>89</v>
@@ -1272,25 +1262,25 @@
         <v>714</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>90</v>
@@ -1306,25 +1296,25 @@
         <v>714</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>90</v>
@@ -1340,25 +1330,25 @@
         <v>714</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>90</v>
@@ -1376,28 +1366,28 @@
         <v>117</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1412,28 +1402,28 @@
         <v>117</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1448,25 +1438,25 @@
         <v>117</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>92</v>
@@ -1482,25 +1472,25 @@
         <v>714</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>90</v>
@@ -1516,13 +1506,13 @@
         <v>341</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>11</v>
@@ -1534,7 +1524,7 @@
         <v>11</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L23" s="3"/>
     </row>
@@ -1550,13 +1540,13 @@
         <v>341</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>11</v>
@@ -1568,7 +1558,7 @@
         <v>11</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L24" s="3"/>
     </row>
@@ -1584,13 +1574,13 @@
         <v>512</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>11</v>
@@ -1602,7 +1592,7 @@
         <v>11</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>91</v>
@@ -1620,13 +1610,13 @@
         <v>512</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>11</v>
@@ -1638,11 +1628,9 @@
         <v>11</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -1656,13 +1644,13 @@
         <v>512</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>11</v>
@@ -1674,11 +1662,9 @@
         <v>11</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
@@ -1692,13 +1678,13 @@
         <v>512</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>11</v>
@@ -1710,11 +1696,9 @@
         <v>11</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
@@ -1728,13 +1712,13 @@
         <v>512</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>11</v>
@@ -1746,11 +1730,9 @@
         <v>11</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -1764,13 +1746,13 @@
         <v>512</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>11</v>
@@ -1782,10 +1764,10 @@
         <v>11</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1800,13 +1782,13 @@
         <v>512</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>11</v>
@@ -1818,7 +1800,7 @@
         <v>11</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L31" s="3"/>
     </row>
@@ -1834,13 +1816,13 @@
         <v>341</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>11</v>
@@ -1852,7 +1834,7 @@
         <v>11</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L32" s="3"/>
     </row>
@@ -1868,13 +1850,13 @@
         <v>341</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>11</v>
@@ -1886,7 +1868,7 @@
         <v>11</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L33" s="3"/>
     </row>
@@ -1902,13 +1884,13 @@
         <v>341</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>11</v>
@@ -1920,7 +1902,7 @@
         <v>11</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L34" s="3"/>
     </row>
@@ -1934,13 +1916,13 @@
         <v>341</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>11</v>
@@ -1952,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>91</v>
@@ -1970,13 +1952,13 @@
         <v>341</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>11</v>
@@ -1988,7 +1970,7 @@
         <v>11</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L36" s="3"/>
     </row>
@@ -2004,13 +1986,13 @@
         <v>117</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>11</v>
@@ -2022,10 +2004,10 @@
         <v>11</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2038,13 +2020,13 @@
         <v>714</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>11</v>
@@ -2056,7 +2038,7 @@
         <v>11</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>91</v>
@@ -2072,13 +2054,13 @@
         <v>714</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>11</v>
@@ -2090,7 +2072,7 @@
         <v>11</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>91</v>
@@ -2106,13 +2088,13 @@
         <v>714</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>11</v>
@@ -2124,7 +2106,7 @@
         <v>11</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>91</v>
@@ -2140,13 +2122,13 @@
         <v>714</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>11</v>
@@ -2158,7 +2140,7 @@
         <v>11</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>90</v>
@@ -2174,13 +2156,13 @@
         <v>714</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>11</v>
@@ -2192,7 +2174,7 @@
         <v>11</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>90</v>
@@ -2208,13 +2190,13 @@
         <v>714</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>11</v>
@@ -2226,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>90</v>
@@ -2242,13 +2224,13 @@
         <v>714</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>11</v>
@@ -2260,7 +2242,7 @@
         <v>11</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>90</v>
@@ -2276,13 +2258,13 @@
         <v>714</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>11</v>
@@ -2294,7 +2276,7 @@
         <v>11</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>90</v>
@@ -2310,13 +2292,13 @@
         <v>714</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>11</v>
@@ -2328,7 +2310,7 @@
         <v>11</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>90</v>
@@ -2344,13 +2326,13 @@
         <v>714</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>11</v>
@@ -2362,7 +2344,7 @@
         <v>11</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>90</v>
@@ -2378,13 +2360,13 @@
         <v>714</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>11</v>
@@ -2396,7 +2378,7 @@
         <v>11</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>90</v>
@@ -2412,13 +2394,13 @@
         <v>714</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>11</v>
@@ -2430,7 +2412,7 @@
         <v>11</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>91</v>
@@ -2446,13 +2428,13 @@
         <v>714</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>11</v>
@@ -2464,7 +2446,7 @@
         <v>11</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>91</v>
@@ -2482,13 +2464,13 @@
         <v>117</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>11</v>
@@ -2500,7 +2482,7 @@
         <v>11</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>91</v>
@@ -2516,13 +2498,13 @@
         <v>117</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>11</v>
@@ -2534,7 +2516,7 @@
         <v>11</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>91</v>
@@ -2552,13 +2534,13 @@
         <v>512</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>11</v>
@@ -2570,11 +2552,9 @@
         <v>11</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>95</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L53" s="3"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -2588,13 +2568,13 @@
         <v>714</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>11</v>
@@ -2606,10 +2586,10 @@
         <v>11</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -2624,10 +2604,10 @@
         <v>512</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>11</v>
@@ -2636,13 +2616,13 @@
         <v>11</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L55" s="3"/>
     </row>
@@ -2658,10 +2638,10 @@
         <v>512</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>11</v>
@@ -2670,13 +2650,13 @@
         <v>11</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L56" s="3"/>
     </row>
@@ -2692,10 +2672,10 @@
         <v>117</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>11</v>
@@ -2704,13 +2684,13 @@
         <v>11</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L57" s="3"/>
     </row>
@@ -2726,10 +2706,10 @@
         <v>177</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>11</v>
@@ -2738,21 +2718,21 @@
         <v>11</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2760,13 +2740,13 @@
         <v>512</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>11</v>
@@ -2778,15 +2758,15 @@
         <v>11</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -2794,13 +2774,13 @@
         <v>314</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>11</v>
@@ -2812,10 +2792,10 @@
         <v>11</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>